<commit_message>
Refactor Credly badge integration to use direct image and badge URLs instead of embed codes.
</commit_message>
<xml_diff>
--- a/files/ResumeAssets.xlsx
+++ b/files/ResumeAssets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Patents &amp; Publications" sheetId="1" state="visible" r:id="rId3"/>
@@ -15,17 +15,17 @@
     <sheet name="WorkProjects" sheetId="5" state="visible" r:id="rId7"/>
     <sheet name="Internships" sheetId="6" state="visible" r:id="rId8"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="120">
   <si>
     <t xml:space="preserve">Type</t>
   </si>
@@ -168,112 +168,13 @@
     <t xml:space="preserve">https://www.coursera.org/account/accomplishments/specialization/certificate/GZ4QPHKSPPEJ</t>
   </si>
   <si>
-    <t xml:space="preserve">Badge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Embed code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AWS Certified Machine Learning – Specialty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div data-iframe-width="150" data-iframe-height="270" data-share-badge-id="0bc048fc-c019-411f-ab6f-1544664ec033" data-share-badge-host="https://www.credly.com"&gt;&lt;/div&gt;&lt;script type="text/javascript" async src="//cdn.credly.com/assets/utilities/embed.js"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div data-iframe-width="150" data-iframe-height="270" data-share-badge-id="407c748f-568d-4aab-97bc-7153f79550f6" data-share-badge-host="https://www.credly.com"&gt;&lt;/div&gt;&lt;script type="text/javascript" async src="//cdn.credly.com/assets/utilities/embed.js"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AWS Certified AI Practitioner Early Adopter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div data-iframe-width="150" data-iframe-height="270" data-share-badge-id="6e3b9311-fc18-47a9-b204-f8ebfac7e154" data-share-badge-host="https://www.credly.com"&gt;&lt;/div&gt;&lt;script type="text/javascript" async src="//cdn.credly.com/assets/utilities/embed.js"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div data-iframe-width="150" data-iframe-height="270" data-share-badge-id="dbe3e6eb-01f9-4f3b-b431-fa887016698e" data-share-badge-host="https://www.credly.com"&gt;&lt;/div&gt;&lt;script type="text/javascript" async src="//cdn.credly.com/assets/utilities/embed.js"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inclusive Mindset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div data-iframe-width="150" data-iframe-height="270" data-share-badge-id="ae2fc8da-312d-486d-ba9c-55981d08dea2" data-share-badge-host="https://www.credly.com"&gt;&lt;/div&gt;&lt;script type="text/javascript" async src="//cdn.credly.com/assets/utilities/embed.js"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digital Acumen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div data-iframe-width="150" data-iframe-height="270" data-share-badge-id="7fad8267-8713-4aff-805c-6f7490198d89" data-share-badge-host="https://www.credly.com"&gt;&lt;/div&gt;&lt;script type="text/javascript" async src="//cdn.credly.com/assets/utilities/embed.js"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Human-Centered Design</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div data-iframe-width="150" data-iframe-height="270" data-share-badge-id="96703463-59fb-4e6d-b281-e0ccdad46461" data-share-badge-host="https://www.credly.com"&gt;&lt;/div&gt;&lt;script type="text/javascript" async src="//cdn.credly.com/assets/utilities/embed.js"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div data-iframe-width="150" data-iframe-height="270" data-share-badge-id="c5987d48-dac8-462d-a6ea-28cf6b72b5fa" data-share-badge-host="https://www.credly.com"&gt;&lt;/div&gt;&lt;script type="text/javascript" async src="//cdn.credly.com/assets/utilities/embed.js"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div data-iframe-width="150" data-iframe-height="270" data-share-badge-id="e6ed7df5-7daf-4240-943c-8ba585985be0" data-share-badge-host="https://www.credly.com"&gt;&lt;/div&gt;&lt;script type="text/javascript" async src="//cdn.credly.com/assets/utilities/embed.js"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Machine Learning with Python</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div data-iframe-width="150" data-iframe-height="270" data-share-badge-id="5569b3c5-0893-480b-8e36-2c751b5276fa" data-share-badge-host="https://www.credly.com"&gt;&lt;/div&gt;&lt;script type="text/javascript" async src="//cdn.credly.com/assets/utilities/embed.js"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Visualization with Python</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div data-iframe-width="150" data-iframe-height="270" data-share-badge-id="67a6bfaa-57e6-4e11-ab19-b6947f33baca" data-share-badge-host="https://www.credly.com"&gt;&lt;/div&gt;&lt;script type="text/javascript" async src="//cdn.credly.com/assets/utilities/embed.js"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Analysis with Python</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div data-iframe-width="150" data-iframe-height="270" data-share-badge-id="cb0eb950-676a-476e-81be-167ae1655eaf" data-share-badge-host="https://www.credly.com"&gt;&lt;/div&gt;&lt;script type="text/javascript" async src="//cdn.credly.com/assets/utilities/embed.js"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Databases and SQL for Data Science</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div data-iframe-width="150" data-iframe-height="270" data-share-badge-id="f09e587c-71ed-4e2b-8785-d7b03013e45f" data-share-badge-host="https://www.credly.com"&gt;&lt;/div&gt;&lt;script type="text/javascript" async src="//cdn.credly.com/assets/utilities/embed.js"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Python for Data Science and AI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div data-iframe-width="150" data-iframe-height="270" data-share-badge-id="58a7097b-f0f4-41dd-9f71-c4c5b1ddb99f" data-share-badge-host="https://www.credly.com"&gt;&lt;/div&gt;&lt;script type="text/javascript" async src="//cdn.credly.com/assets/utilities/embed.js"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Science Methodology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div data-iframe-width="150" data-iframe-height="270" data-share-badge-id="d6b09c86-3730-433c-93be-fc06ea4852e3" data-share-badge-host="https://www.credly.com"&gt;&lt;/div&gt;&lt;script type="text/javascript" async src="//cdn.credly.com/assets/utilities/embed.js"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tools for Data Science</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div data-iframe-width="150" data-iframe-height="270" data-share-badge-id="47562298-1cd3-492e-8c5d-6517f1873638" data-share-badge-host="https://www.credly.com"&gt;&lt;/div&gt;&lt;script type="text/javascript" async src="//cdn.credly.com/assets/utilities/embed.js"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Science Orientation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div data-iframe-width="150" data-iframe-height="270" data-share-badge-id="4ce08ed3-114f-4150-b280-b366721cf3e4" data-share-badge-host="https://www.credly.com"&gt;&lt;/div&gt;&lt;script type="text/javascript" async src="//cdn.credly.com/assets/utilities/embed.js"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADAA 2017 Participant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div data-iframe-width="150" data-iframe-height="270" data-share-badge-id="6815f7ab-eeda-46ca-8f26-fd219b4076c8" data-share-badge-host="https://www.credly.com"&gt;&lt;/div&gt;&lt;script type="text/javascript" async src="//cdn.credly.com/assets/utilities/embed.js"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IBM Blockchain Essentials</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div data-iframe-width="150" data-iframe-height="270" data-share-badge-id="1b755f40-0aed-45a4-b8df-2f087d82f57c" data-share-badge-host="https://www.credly.com"&gt;&lt;/div&gt;&lt;script type="text/javascript" async src="//cdn.credly.com/assets/utilities/embed.js"&gt;&lt;/script&gt;</t>
+    <t xml:space="preserve">ProfileURL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.credly.com/users/bibhash-mitra/badges.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.credly.com/users/bibhash-mitra-old/badges.json</t>
   </si>
   <si>
     <t xml:space="preserve">RoleId</t>
@@ -500,9 +401,9 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="4">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -522,19 +423,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -579,21 +467,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -691,14 +571,17 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
+                <a:shade val="94000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -791,7 +674,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.43359375" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -804,7 +687,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
@@ -815,7 +698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>3</v>
       </c>
@@ -826,7 +709,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>3</v>
       </c>
@@ -837,7 +720,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>3</v>
       </c>
@@ -848,7 +731,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>3</v>
       </c>
@@ -859,7 +742,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>14</v>
       </c>
@@ -871,16 +754,8 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://patents.google.com/patent/US20250252335A1"/>
-    <hyperlink ref="C3" r:id="rId2" display="https://patents.google.com/patent/US20250165824A1"/>
-    <hyperlink ref="C4" r:id="rId3" display="https://patents.google.com/patent/US20250104559A1"/>
-    <hyperlink ref="C5" r:id="rId4" display="https://patents.google.com/patent/US20220406403A1/en?oq=20220406403"/>
-    <hyperlink ref="C6" r:id="rId5" display="https://patents.google.com/patent/US20230115171A1/en?oq=US20230115171A1"/>
-    <hyperlink ref="C7" r:id="rId6" display="https://arc.aiaa.org/doi/10.2514/6.2019-1166"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -900,7 +775,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.43359375" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -913,7 +788,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>18</v>
       </c>
@@ -924,7 +799,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>18</v>
       </c>
@@ -935,7 +810,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>18</v>
       </c>
@@ -946,7 +821,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>25</v>
       </c>
@@ -957,7 +832,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>28</v>
       </c>
@@ -968,7 +843,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>31</v>
       </c>
@@ -979,7 +854,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="16.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>34</v>
       </c>
@@ -990,7 +865,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>34</v>
       </c>
@@ -1001,7 +876,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="16.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>34</v>
       </c>
@@ -1012,7 +887,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="16.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>34</v>
       </c>
@@ -1023,7 +898,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="16.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>34</v>
       </c>
@@ -1034,7 +909,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="16.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>34</v>
       </c>
@@ -1046,22 +921,8 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://cp.certmetrics.com/amazon/en/public/verify/credential/e7b1ab967c3247bc8b8477a0f0da0019"/>
-    <hyperlink ref="C3" r:id="rId2" display="https://cp.certmetrics.com/amazon/en/public/verify/credential/2c6a95f7989046d0a5bcc4352e351e5d"/>
-    <hyperlink ref="C4" r:id="rId3" display="https://cp.certmetrics.com/amazon/en/public/verify/credential/2d038a52d6a8441190b429a55d87c7d4"/>
-    <hyperlink ref="C5" r:id="rId4" display="https://learn.microsoft.com/api/credentials/share/en-us/BibhashMitra/90AEC65E5A4A8FFD?sharingId=39DEA8414B60265"/>
-    <hyperlink ref="C6" r:id="rId5" display="https://www.credly.com/badges/c5987d48-dac8-462d-a6ea-28cf6b72b5fa/public_url"/>
-    <hyperlink ref="C7" r:id="rId6" display="https://www.credly.com/badges/e6ed7df5-7daf-4240-943c-8ba585985be0/public_url"/>
-    <hyperlink ref="C8" r:id="rId7" display="https://www.coursera.org/account/accomplishments/specialization/certificate/7YA55DLQFVQ4"/>
-    <hyperlink ref="C9" r:id="rId8" display="https://www.coursera.org/account/accomplishments/specialization/8XBN32GQLH7B"/>
-    <hyperlink ref="C10" r:id="rId9" display="https://www.coursera.org/account/accomplishments/specialization/certificate/62QBRLAXMQPY"/>
-    <hyperlink ref="C11" r:id="rId10" display="https://www.coursera.org/account/accomplishments/specialization/certificate/B69K4TTFL7D5"/>
-    <hyperlink ref="C12" r:id="rId11" display="https://www.coursera.org/account/accomplishments/specialization/certificate/UF4HUSYMR7GW"/>
-    <hyperlink ref="C13" r:id="rId12" display="https://www.coursera.org/account/accomplishments/specialization/certificate/GZ4QPHKSPPEJ"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -1075,177 +936,35 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.43359375" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>82</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" display="https://www.credly.com/users/bibhash-mitra-old/badges.json"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -1265,103 +984,96 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="70.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.84"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.43359375" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>98</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>102</v>
+        <v>69</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -1377,240 +1089,235 @@
   </sheetPr>
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="150.84"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.43359375" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="27.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>107</v>
+        <v>73</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>109</v>
+        <v>55</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="27.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>55</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>112</v>
+        <v>79</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="27.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>115</v>
+        <v>81</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>117</v>
+        <v>60</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="27.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>60</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>120</v>
+        <v>60</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>87</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>63</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>127</v>
+        <v>63</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>96</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>131</v>
+        <v>66</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>133</v>
+      <c r="C15" s="0" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>135</v>
+        <v>66</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>137</v>
+        <v>66</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>138</v>
+        <v>105</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="39.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="42.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>140</v>
+        <v>66</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>107</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>141</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -1630,68 +1337,62 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="25.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="150.84"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.43359375" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>144</v>
+        <v>111</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>145</v>
+        <v>112</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>146</v>
+        <v>113</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>147</v>
+        <v>114</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>148</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>149</v>
+        <v>116</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>145</v>
+        <v>112</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>150</v>
+        <v>117</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>151</v>
+        <v>118</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>